<commit_message>
Set backend for driver
</commit_message>
<xml_diff>
--- a/assets/menu_data.xlsx
+++ b/assets/menu_data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AE8B72-A3D8-4F46-9EA0-D81D06C315B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="21795" windowHeight="12975" activeTab="1"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="store" sheetId="1" r:id="rId1"/>
@@ -130,9 +131,6 @@
     <t>The classic fried chicken that made KFC famous</t>
   </si>
   <si>
-    <t>https://kfc.com/images/products/large/kfc.original.recipe.chicken.large.png</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -148,9 +146,6 @@
     <t>Spicy chicken fillet in a sesame bun</t>
   </si>
   <si>
-    <t>https://kfc.com/images/products/large/kfc.zinger.burger.large.png</t>
-  </si>
-  <si>
     <t>Spicy, Popular</t>
   </si>
   <si>
@@ -163,9 +158,6 @@
     <t>Espresso with steamed milk and caramel flavor</t>
   </si>
   <si>
-    <t>https://starbucks.com/images/products/large/caramel.macchiato.large.png</t>
-  </si>
-  <si>
     <t>Popular, Caramel</t>
   </si>
   <si>
@@ -175,9 +167,6 @@
     <t>Rich and bold espresso shot</t>
   </si>
   <si>
-    <t>https://starbucks.com/images/products/large/espresso.large.png</t>
-  </si>
-  <si>
     <t>Hot</t>
   </si>
   <si>
@@ -190,18 +179,12 @@
     <t>Two beef patties with special sauce</t>
   </si>
   <si>
-    <t>https://mcdonalds.com/images/products/large/big.mac.large.png</t>
-  </si>
-  <si>
     <t>McChicken</t>
   </si>
   <si>
     <t>Crispy chicken sandwich with mayo</t>
   </si>
   <si>
-    <t>https://mcdonalds.com/images/products/large/mcchicken.large.png</t>
-  </si>
-  <si>
     <t>Popular</t>
   </si>
   <si>
@@ -211,9 +194,6 @@
     <t>Classic glazed donut</t>
   </si>
   <si>
-    <t>https://dunkin.com/images/products/large/glazed.donut.large.png</t>
-  </si>
-  <si>
     <t>Donut</t>
   </si>
   <si>
@@ -223,9 +203,6 @@
     <t>Freshly brewed coffee</t>
   </si>
   <si>
-    <t>https://dunkin.com/images/products/large/dunkin.coffee.large.png</t>
-  </si>
-  <si>
     <t>Classic, Popular</t>
   </si>
   <si>
@@ -235,28 +212,52 @@
     <t>Flame-grilled beef patty with fresh veggies</t>
   </si>
   <si>
-    <t>https://burgerking.com/images/products/large/whopper.large.png</t>
-  </si>
-  <si>
     <t>Chicken Fries</t>
   </si>
   <si>
     <t>Crispy chicken fries with dipping sauce</t>
   </si>
   <si>
-    <t>https://burgerking.com/images/products/large/chicken.fries.large.png</t>
-  </si>
-  <si>
     <t>Popular, Snack</t>
   </si>
   <si>
     <t>Snack</t>
+  </si>
+  <si>
+    <t>https://static.order.kfcku.com/images/items/lg/5587.jpg?v=gqGmqL</t>
+  </si>
+  <si>
+    <t>https://brand-uk.assets.kfc.co.uk/2023-10/KFC4317~39047_W8_23_ZINGER_BURGER_MEAL_1200x800.jpg?VersionId=APSJn8Jb5_jlGX1O3FEjwHadslkrlfXa</t>
+  </si>
+  <si>
+    <t>https://www.shutterstock.com/image-photo/brno-czechia-06162023-starbucks-coffee-600nw-2320284399.jpg</t>
+  </si>
+  <si>
+    <t>https://www.starbucks.co.th/stb-media/2020/08/1.Espresso-1080.png</t>
+  </si>
+  <si>
+    <t>https://s7d1.scene7.com/is/image/mcdonalds/Header_BigMac_832x472:1-3-product-tile-desktop?wid=763&amp;hei=472&amp;dpr=off</t>
+  </si>
+  <si>
+    <t>https://www.sidechef.com/recipe/b4496acb-32b7-4b27-8d91-b6e7a3c21218.jpg?d=1408x1120</t>
+  </si>
+  <si>
+    <t>https://www.keyingredient.com/uploads/media/be/80/8316c8fb81a8cb68a15047c2748cf376d525.jpg?1560436606</t>
+  </si>
+  <si>
+    <t>https://www.shape.com/thmb/DJKMBoJgTF_lfPnzAI4cnLhGD5w=/1500x0/filters:no_upscale():max_bytes(150000):strip_icc()/hot-coffee-8079cd4654e84c07924b12d4f78b2cb5.jpg</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/burgerking/images/3/3c/Whopper_JR.jpg/revision/latest?cb=20190619155429</t>
+  </si>
+  <si>
+    <t>https://i0.wp.com/www.theimpulsivebuy.com/wordpress/wp-content/uploads/2023/10/bkghopepchickfries.jpg?fit=1200%2C1200&amp;ssl=1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -578,21 +579,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.265625" customWidth="1"/>
+    <col min="4" max="4" width="8.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -606,7 +607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -620,7 +621,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -634,7 +635,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -648,7 +649,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -662,7 +663,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -676,7 +677,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -696,28 +697,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="144.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -752,7 +753,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -787,7 +788,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -822,7 +823,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -835,20 +836,20 @@
       <c r="D4" t="s">
         <v>35</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" t="s">
         <v>36</v>
-      </c>
-      <c r="F4" t="s">
-        <v>37</v>
       </c>
       <c r="G4">
         <v>15</v>
       </c>
       <c r="H4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s">
         <v>38</v>
-      </c>
-      <c r="I4" t="s">
-        <v>39</v>
       </c>
       <c r="J4">
         <v>4.7</v>
@@ -857,7 +858,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -865,25 +866,25 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
         <v>40</v>
       </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>42</v>
+      <c r="E5" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G5">
         <v>5.5</v>
       </c>
       <c r="H5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J5">
         <v>4.5</v>
@@ -892,7 +893,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -900,13 +901,13 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
@@ -915,7 +916,7 @@
         <v>4.5</v>
       </c>
       <c r="H6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I6" t="s">
         <v>11</v>
@@ -927,7 +928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -935,22 +936,22 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G7">
         <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
@@ -962,7 +963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -970,25 +971,25 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" t="s">
-        <v>56</v>
+        <v>51</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G8">
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J8">
         <v>4.7</v>
@@ -997,7 +998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1005,25 +1006,25 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9">
         <v>3.5</v>
       </c>
       <c r="H9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="I9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J9">
         <v>4.5999999999999996</v>
@@ -1032,7 +1033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1040,25 +1041,25 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" t="s">
-        <v>63</v>
+        <v>56</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10">
         <v>1.5</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="I10" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="J10">
         <v>4.5</v>
@@ -1067,7 +1068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1075,13 +1076,13 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
@@ -1090,7 +1091,7 @@
         <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
@@ -1102,7 +1103,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1110,25 +1111,25 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" t="s">
-        <v>71</v>
+        <v>62</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G12">
         <v>6</v>
       </c>
       <c r="H12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J12">
         <v>4.8</v>
@@ -1137,7 +1138,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1145,25 +1146,25 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" t="s">
-        <v>74</v>
+        <v>64</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13">
         <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="I13" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="J13">
         <v>4.5999999999999996</v>
@@ -1173,6 +1174,18 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{7251F47A-49C6-477A-B16A-7023C162F7CA}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{5A11F7A2-CE6E-4C23-BBA8-0EC2F008EFB5}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{2391135A-18F3-4D58-94DF-52BF54AACCA4}"/>
+    <hyperlink ref="E7" r:id="rId4" xr:uid="{10202B0D-0CB0-4314-8BF4-A964F891DC8C}"/>
+    <hyperlink ref="E8" r:id="rId5" xr:uid="{D830AD51-F55E-4BD4-BDE1-D2545F0070EC}"/>
+    <hyperlink ref="E9" r:id="rId6" xr:uid="{681EE41A-0F5D-4377-8214-C02E2F14858F}"/>
+    <hyperlink ref="E10" r:id="rId7" xr:uid="{A442ACE6-7E43-46F6-B519-F997695D84FA}"/>
+    <hyperlink ref="E11" r:id="rId8" xr:uid="{6B1FEE4D-A926-4910-944E-03861D105153}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{A9A4F521-53A3-495C-845A-FB180CF6EAF6}"/>
+    <hyperlink ref="E13" r:id="rId10" xr:uid="{D43DEE4F-1EDC-4D33-973E-3958EB225A5E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Integrate My Account page to database
</commit_message>
<xml_diff>
--- a/assets/menu_data.xlsx
+++ b/assets/menu_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AE8B72-A3D8-4F46-9EA0-D81D06C315B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F38C568-21B8-4C38-8362-BA2D44E60D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="store" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="78">
   <si>
     <t>name</t>
   </si>
@@ -68,9 +68,6 @@
     <t>image</t>
   </si>
   <si>
-    <t>temp.jpg</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -95,27 +92,15 @@
     <t>Starbucks</t>
   </si>
   <si>
-    <t>starbucks.jpg</t>
-  </si>
-  <si>
     <t>McDonald's</t>
   </si>
   <si>
-    <t>mcdonalds.jpg</t>
-  </si>
-  <si>
     <t>Dunkin'</t>
   </si>
   <si>
-    <t>dunkin.jpg</t>
-  </si>
-  <si>
     <t>Burger King</t>
   </si>
   <si>
-    <t>burger_king.jpg</t>
-  </si>
-  <si>
     <t>A rich, aromatic coffee blend with a smooth finish</t>
   </si>
   <si>
@@ -252,6 +237,24 @@
   </si>
   <si>
     <t>https://i0.wp.com/www.theimpulsivebuy.com/wordpress/wp-content/uploads/2023/10/bkghopepchickfries.jpg?fit=1200%2C1200&amp;ssl=1</t>
+  </si>
+  <si>
+    <t>https://sebenarnya.my/wp-content/uploads/2017/02/old-town-coffee-1.jpg</t>
+  </si>
+  <si>
+    <t>https://media-cdn.tripadvisor.com/media/photo-s/06/a4/b3/f2/kfc-kentucky-fried-chicken.jpg</t>
+  </si>
+  <si>
+    <t>https://media-cdn.tripadvisor.com/media/photo-s/1a/9f/86/0f/caption.jpg</t>
+  </si>
+  <si>
+    <t>https://www.thedailymeal.com/img/gallery/avoid-these-14-mistakes-when-ordering-at-mcdonalds/intro-1680098756.jpg</t>
+  </si>
+  <si>
+    <t>https://proriat-franchise.com/wp-content/uploads/2021/08/161632.jpg</t>
+  </si>
+  <si>
+    <t>https://media-cdn.tripadvisor.com/media/photo-s/0e/47/81/3e/outside.jpg</t>
   </si>
 </sst>
 </file>
@@ -582,20 +585,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.265625" customWidth="1"/>
-    <col min="4" max="4" width="8.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.59765625" customWidth="1"/>
+    <col min="3" max="3" width="97.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -614,8 +617,8 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
+      <c r="C2" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -626,13 +629,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -640,10 +643,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -654,13 +657,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -668,10 +671,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -682,16 +685,24 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{F33E480A-E57D-4A36-9CC7-FBCCD5A71FD0}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{2EA4466C-53AA-46ED-B6A7-B5E09B529030}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{A1DD3313-E52C-4B70-BC31-A7A4A44D6220}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{A8F964A8-02D4-42D0-AA40-B9736BB51452}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{0E5F8515-526A-4418-A5E0-88051D4BCA14}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{B9574C12-5C87-465B-81D8-6B4F2BD732AA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -700,7 +711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -720,10 +731,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -764,10 +775,10 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -776,10 +787,10 @@
         <v>9.9</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2">
         <v>4.5999999999999996</v>
@@ -799,10 +810,10 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -811,7 +822,7 @@
         <v>12.9</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
@@ -831,25 +842,25 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G4">
         <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J4">
         <v>4.7</v>
@@ -866,25 +877,25 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G5">
         <v>5.5</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J5">
         <v>4.5</v>
@@ -901,13 +912,13 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
@@ -916,7 +927,7 @@
         <v>4.5</v>
       </c>
       <c r="H6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="I6" t="s">
         <v>11</v>
@@ -936,22 +947,22 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G7">
         <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
@@ -971,25 +982,25 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G8">
         <v>5</v>
       </c>
       <c r="H8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" t="s">
         <v>37</v>
-      </c>
-      <c r="I8" t="s">
-        <v>42</v>
       </c>
       <c r="J8">
         <v>4.7</v>
@@ -1006,25 +1017,25 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G9">
         <v>3.5</v>
       </c>
       <c r="H9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J9">
         <v>4.5999999999999996</v>
@@ -1041,25 +1052,25 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G10">
         <v>1.5</v>
       </c>
       <c r="H10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="J10">
         <v>4.5</v>
@@ -1076,13 +1087,13 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
@@ -1091,7 +1102,7 @@
         <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
@@ -1111,25 +1122,25 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G12">
         <v>6</v>
       </c>
       <c r="H12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" t="s">
         <v>37</v>
-      </c>
-      <c r="I12" t="s">
-        <v>42</v>
       </c>
       <c r="J12">
         <v>4.8</v>
@@ -1146,25 +1157,25 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G13">
         <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="I13" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="J13">
         <v>4.5999999999999996</v>

</xml_diff>

<commit_message>
Integrate Map API to store location on database
</commit_message>
<xml_diff>
--- a/assets/menu_data.xlsx
+++ b/assets/menu_data.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7184644D-703A-40CA-A8BC-484561F465A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="21795" windowHeight="12975"/>
   </bookViews>
   <sheets>
     <sheet name="store" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="220">
   <si>
     <t>name</t>
   </si>
@@ -675,12 +674,18 @@
   </si>
   <si>
     <t>Ice 30%,Ice 50%,Full Ice</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1002,21 +1007,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.59765625" customWidth="1"/>
-    <col min="3" max="3" width="97.9296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="98" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1029,8 +1034,14 @@
       <c r="D1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1043,8 +1054,14 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E2">
+        <v>3.1390030000000002</v>
+      </c>
+      <c r="F2">
+        <v>101.68685499999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1057,8 +1074,14 @@
       <c r="D3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E3">
+        <v>3.1341199999999998</v>
+      </c>
+      <c r="F3">
+        <v>101.68653</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1071,8 +1094,14 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E4">
+        <v>3.1352799999999998</v>
+      </c>
+      <c r="F4">
+        <v>101.6871</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1085,8 +1114,14 @@
       <c r="D5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E5">
+        <v>3.13428</v>
+      </c>
+      <c r="F5">
+        <v>101.68810000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1099,8 +1134,14 @@
       <c r="D6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E6">
+        <v>3.13571</v>
+      </c>
+      <c r="F6">
+        <v>101.6961</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1113,43 +1154,50 @@
       <c r="D7" t="s">
         <v>16</v>
       </c>
+      <c r="E7">
+        <v>3.1360100000000002</v>
+      </c>
+      <c r="F7">
+        <v>101.68899999999999</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{F33E480A-E57D-4A36-9CC7-FBCCD5A71FD0}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{2EA4466C-53AA-46ED-B6A7-B5E09B529030}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{A1DD3313-E52C-4B70-BC31-A7A4A44D6220}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{A8F964A8-02D4-42D0-AA40-B9736BB51452}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{0E5F8515-526A-4418-A5E0-88051D4BCA14}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{B9574C12-5C87-465B-81D8-6B4F2BD732AA}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
-    <col min="5" max="5" width="144.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="144.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="10" max="10" width="5.3984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1184,7 +1232,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1219,7 +1267,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1254,7 +1302,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1289,7 +1337,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1324,7 +1372,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1359,7 +1407,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1394,7 +1442,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1429,7 +1477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1464,7 +1512,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1499,7 +1547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1534,7 +1582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1569,7 +1617,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1604,7 +1652,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1639,7 +1687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1674,7 +1722,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1709,7 +1757,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1744,7 +1792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1779,7 +1827,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1814,7 +1862,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1849,7 +1897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1884,7 +1932,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1919,7 +1967,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1954,7 +2002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1989,7 +2037,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2024,7 +2072,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2059,7 +2107,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2094,7 +2142,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2129,7 +2177,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2164,7 +2212,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2199,7 +2247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2234,7 +2282,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2269,7 +2317,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2304,7 +2352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2339,7 +2387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2374,7 +2422,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2409,7 +2457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2444,7 +2492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2479,7 +2527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2514,7 +2562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2549,7 +2597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2584,7 +2632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2619,7 +2667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2654,7 +2702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2689,7 +2737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2724,7 +2772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2759,7 +2807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2794,7 +2842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2829,7 +2877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2864,7 +2912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2899,7 +2947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2934,7 +2982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2969,7 +3017,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3004,7 +3052,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3039,7 +3087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3074,7 +3122,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3109,7 +3157,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3144,7 +3192,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3179,7 +3227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3214,7 +3262,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3249,7 +3297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3286,17 +3334,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E12" r:id="rId1" xr:uid="{7251F47A-49C6-477A-B16A-7023C162F7CA}"/>
-    <hyperlink ref="E13" r:id="rId2" xr:uid="{5A11F7A2-CE6E-4C23-BBA8-0EC2F008EFB5}"/>
-    <hyperlink ref="E22" r:id="rId3" xr:uid="{2391135A-18F3-4D58-94DF-52BF54AACCA4}"/>
-    <hyperlink ref="E23" r:id="rId4" xr:uid="{10202B0D-0CB0-4314-8BF4-A964F891DC8C}"/>
-    <hyperlink ref="E32" r:id="rId5" xr:uid="{D830AD51-F55E-4BD4-BDE1-D2545F0070EC}"/>
-    <hyperlink ref="E33" r:id="rId6" xr:uid="{681EE41A-0F5D-4377-8214-C02E2F14858F}"/>
-    <hyperlink ref="E42" r:id="rId7" xr:uid="{A442ACE6-7E43-46F6-B519-F997695D84FA}"/>
-    <hyperlink ref="E43" r:id="rId8" xr:uid="{6B1FEE4D-A926-4910-944E-03861D105153}"/>
-    <hyperlink ref="E52" r:id="rId9" xr:uid="{A9A4F521-53A3-495C-845A-FB180CF6EAF6}"/>
-    <hyperlink ref="E53" r:id="rId10" xr:uid="{D43DEE4F-1EDC-4D33-973E-3958EB225A5E}"/>
-    <hyperlink ref="E14" r:id="rId11" xr:uid="{3D6A1DC7-DB38-406A-AFFE-FD190C626B61}"/>
+    <hyperlink ref="E12" r:id="rId1"/>
+    <hyperlink ref="E13" r:id="rId2"/>
+    <hyperlink ref="E22" r:id="rId3"/>
+    <hyperlink ref="E23" r:id="rId4"/>
+    <hyperlink ref="E32" r:id="rId5"/>
+    <hyperlink ref="E33" r:id="rId6"/>
+    <hyperlink ref="E42" r:id="rId7"/>
+    <hyperlink ref="E43" r:id="rId8"/>
+    <hyperlink ref="E52" r:id="rId9"/>
+    <hyperlink ref="E53" r:id="rId10"/>
+    <hyperlink ref="E14" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>